<commit_message>
Data.xlsx deleted. Data (1).xlxs renamed to Data.xlsx
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,18 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nemanja\Desktop\finalProject\demoYoMealsTest\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487037FF-02E4-4286-9DB3-3014B7945F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3CD62E05-3796-467B-A016-3514B34A0F8E}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Meal Search Results" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Meals" sheetId="2" r:id="rId5"/>
+    <sheet name="Meal Search Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Meals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>LOCATION</t>
   </si>
@@ -114,6 +134,9 @@
   </si>
   <si>
     <t>MEAL URL</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
   </si>
   <si>
     <t>http://demo.yo-meals.com/meal/chicken-fried-steak-tostada</t>
@@ -134,27 +157,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-    </font>
-    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,7 +189,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -172,100 +199,187 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,27 +520,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D125064-A80C-4E0B-B62B-0471756023FC}">
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.86"/>
-    <col customWidth="1" min="2" max="2" width="25.86"/>
-    <col customWidth="1" min="3" max="3" width="22.29"/>
-    <col customWidth="1" min="4" max="4" width="19.43"/>
-    <col customWidth="1" min="5" max="5" width="18.71"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -445,7 +563,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -460,7 +578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -468,7 +586,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -477,7 +595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -485,13 +603,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -499,10 +617,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -510,7 +628,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
@@ -519,7 +637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -527,7 +645,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
@@ -593,115 +711,89 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22">
-      <c r="B22" s="5"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{ABF6864D-91D5-4987-B515-0CF051E49C55}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{647C1E83-E788-48CD-913E-2CB745EEA633}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{7FCE4B8F-8D04-49D8-87A4-E26D56159857}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{FB4BAD4A-0181-45E6-BB2D-BB527CB7BF9A}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{A5AAFA96-F987-42D6-800C-6D2643080375}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{F268432D-FCF2-448D-AAE6-0CFD65E47FB9}"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F997C670-218A-4B27-BB36-4851FCE75098}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="56.29"/>
+    <col min="1" max="1" width="49.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>38</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A5"/>
-    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CB10236E-DA32-4AC3-BCAF-412026398467}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{9CB9EE5E-B01F-446C-83B8-70A318877444}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{AD108ABD-8727-4280-8CA2-05CA34657092}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{242AFD57-95B3-454A-97A7-628719DD3235}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{F9D3D588-97B7-4927-B9ED-6F25AD97EB4F}"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>